<commit_message>
add additional queries for comparison
</commit_message>
<xml_diff>
--- a/Reg_Season_23_24/SQL/Comparison/Results/2324_team_totals.xlsx
+++ b/Reg_Season_23_24/SQL/Comparison/Results/2324_team_totals.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f8aab243d6baed32/Desktop/Lighthouse/After/NHL-Stats/Reg_Season_23_24/SQL/Comparison/Results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="8_{B10C8C40-B89D-4EA1-A5BB-0B175071704C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C5A95FFC-0E27-448C-BC65-61B27DE02F8F}"/>
+  <xr:revisionPtr revIDLastSave="28" documentId="8_{B10C8C40-B89D-4EA1-A5BB-0B175071704C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5FAC646F-04FE-4FD8-AA94-380FE893F49A}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{91A05544-62E1-4397-9928-AFA81468F948}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{91A05544-62E1-4397-9928-AFA81468F948}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
   <si>
     <t>team</t>
   </si>
@@ -162,9 +162,6 @@
   </si>
   <si>
     <t>avg_save_perc</t>
-  </si>
-  <si>
-    <t>s</t>
   </si>
 </sst>
 </file>
@@ -217,6 +214,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -536,29 +537,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A042EED6-B83D-42EA-BDDE-49CE7D21CC9E}">
-  <dimension ref="A1:Q33"/>
+  <dimension ref="A1:J33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q14" sqref="Q14"/>
+      <selection activeCell="O9" sqref="O9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="5.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.21875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.88671875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.33203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.21875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.5546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.5546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.21875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.44140625" customWidth="1"/>
+    <col min="3" max="3" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9" customWidth="1"/>
+    <col min="7" max="7" width="14.88671875" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="17.88671875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -589,14 +587,8 @@
       <c r="J1" t="s">
         <v>41</v>
       </c>
-      <c r="K1" t="s">
-        <v>1</v>
-      </c>
-      <c r="L1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -613,7 +605,7 @@
         <v>2163</v>
       </c>
       <c r="F2">
-        <v>1044</v>
+        <v>1064</v>
       </c>
       <c r="G2">
         <v>502</v>
@@ -627,14 +619,8 @@
       <c r="J2">
         <v>0.89</v>
       </c>
-      <c r="K2">
-        <v>0</v>
-      </c>
-      <c r="L2">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -651,7 +637,7 @@
         <v>2022</v>
       </c>
       <c r="F3">
-        <v>803</v>
+        <v>805</v>
       </c>
       <c r="G3">
         <v>474</v>
@@ -665,14 +651,8 @@
       <c r="J3">
         <v>0.89900000000000002</v>
       </c>
-      <c r="K3">
-        <v>0</v>
-      </c>
-      <c r="L3">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -689,7 +669,7 @@
         <v>2391</v>
       </c>
       <c r="F4">
-        <v>752</v>
+        <v>754</v>
       </c>
       <c r="G4">
         <v>516</v>
@@ -703,14 +683,8 @@
       <c r="J4">
         <v>0.89800000000000002</v>
       </c>
-      <c r="K4">
-        <v>0</v>
-      </c>
-      <c r="L4">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -727,7 +701,7 @@
         <v>2483</v>
       </c>
       <c r="F5">
-        <v>769</v>
+        <v>777</v>
       </c>
       <c r="G5">
         <v>542</v>
@@ -741,14 +715,8 @@
       <c r="J5">
         <v>0.91400000000000003</v>
       </c>
-      <c r="K5">
-        <v>0</v>
-      </c>
-      <c r="L5">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -765,7 +733,7 @@
         <v>2732</v>
       </c>
       <c r="F6">
-        <v>663</v>
+        <v>669</v>
       </c>
       <c r="G6">
         <v>621</v>
@@ -779,14 +747,8 @@
       <c r="J6">
         <v>0.88700000000000001</v>
       </c>
-      <c r="K6">
-        <v>0</v>
-      </c>
-      <c r="L6">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>11</v>
       </c>
@@ -803,7 +765,7 @@
         <v>2285</v>
       </c>
       <c r="F7">
-        <v>605</v>
+        <v>607</v>
       </c>
       <c r="G7">
         <v>517</v>
@@ -817,14 +779,8 @@
       <c r="J7">
         <v>0.89200000000000002</v>
       </c>
-      <c r="K7">
-        <v>0</v>
-      </c>
-      <c r="L7">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>12</v>
       </c>
@@ -841,7 +797,7 @@
         <v>2404</v>
       </c>
       <c r="F8">
-        <v>704</v>
+        <v>716</v>
       </c>
       <c r="G8">
         <v>621</v>
@@ -855,14 +811,8 @@
       <c r="J8">
         <v>0.88200000000000001</v>
       </c>
-      <c r="K8">
-        <v>0</v>
-      </c>
-      <c r="L8">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>13</v>
       </c>
@@ -893,14 +843,8 @@
       <c r="J9">
         <v>0.89500000000000002</v>
       </c>
-      <c r="K9">
-        <v>0</v>
-      </c>
-      <c r="L9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>14</v>
       </c>
@@ -931,14 +875,8 @@
       <c r="J10">
         <v>0.89700000000000002</v>
       </c>
-      <c r="K10">
-        <v>0</v>
-      </c>
-      <c r="L10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>15</v>
       </c>
@@ -955,7 +893,7 @@
         <v>2588</v>
       </c>
       <c r="F11">
-        <v>536</v>
+        <v>540</v>
       </c>
       <c r="G11">
         <v>560</v>
@@ -969,14 +907,8 @@
       <c r="J11">
         <v>0.89500000000000002</v>
       </c>
-      <c r="K11">
-        <v>0</v>
-      </c>
-      <c r="L11">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>16</v>
       </c>
@@ -993,7 +925,7 @@
         <v>2336</v>
       </c>
       <c r="F12">
-        <v>680</v>
+        <v>686</v>
       </c>
       <c r="G12">
         <v>457</v>
@@ -1007,14 +939,8 @@
       <c r="J12">
         <v>0.90300000000000002</v>
       </c>
-      <c r="K12">
-        <v>0</v>
-      </c>
-      <c r="L12">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>17</v>
       </c>
@@ -1031,7 +957,7 @@
         <v>2750</v>
       </c>
       <c r="F13">
-        <v>760</v>
+        <v>762</v>
       </c>
       <c r="G13">
         <v>707</v>
@@ -1045,14 +971,8 @@
       <c r="J13">
         <v>0.90600000000000003</v>
       </c>
-      <c r="K13">
-        <v>0</v>
-      </c>
-      <c r="L13">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>18</v>
       </c>
@@ -1069,7 +989,7 @@
         <v>2763</v>
       </c>
       <c r="F14">
-        <v>1100</v>
+        <v>1104</v>
       </c>
       <c r="G14">
         <v>564</v>
@@ -1083,17 +1003,8 @@
       <c r="J14">
         <v>0.90900000000000003</v>
       </c>
-      <c r="K14">
-        <v>0</v>
-      </c>
-      <c r="L14">
-        <v>4</v>
-      </c>
-      <c r="Q14" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>19</v>
       </c>
@@ -1110,7 +1021,7 @@
         <v>2587</v>
       </c>
       <c r="F15">
-        <v>687</v>
+        <v>693</v>
       </c>
       <c r="G15">
         <v>424</v>
@@ -1124,14 +1035,8 @@
       <c r="J15">
         <v>0.90200000000000002</v>
       </c>
-      <c r="K15">
-        <v>0</v>
-      </c>
-      <c r="L15">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>20</v>
       </c>
@@ -1148,7 +1053,7 @@
         <v>2439</v>
       </c>
       <c r="F16">
-        <v>908</v>
+        <v>910</v>
       </c>
       <c r="G16">
         <v>497</v>
@@ -1162,14 +1067,8 @@
       <c r="J16">
         <v>0.89600000000000002</v>
       </c>
-      <c r="K16">
-        <v>0</v>
-      </c>
-      <c r="L16">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>21</v>
       </c>
@@ -1186,7 +1085,7 @@
         <v>2100</v>
       </c>
       <c r="F17">
-        <v>734</v>
+        <v>742</v>
       </c>
       <c r="G17">
         <v>463</v>
@@ -1200,14 +1099,8 @@
       <c r="J17">
         <v>0.89700000000000002</v>
       </c>
-      <c r="K17">
-        <v>0</v>
-      </c>
-      <c r="L17">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>22</v>
       </c>
@@ -1238,14 +1131,8 @@
       <c r="J18">
         <v>0.89500000000000002</v>
       </c>
-      <c r="K18">
-        <v>0</v>
-      </c>
-      <c r="L18">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>23</v>
       </c>
@@ -1262,7 +1149,7 @@
         <v>2488</v>
       </c>
       <c r="F19">
-        <v>729</v>
+        <v>731</v>
       </c>
       <c r="G19">
         <v>651</v>
@@ -1276,14 +1163,8 @@
       <c r="J19">
         <v>0.90900000000000003</v>
       </c>
-      <c r="K19">
-        <v>0</v>
-      </c>
-      <c r="L19">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>24</v>
       </c>
@@ -1300,7 +1181,7 @@
         <v>2470</v>
       </c>
       <c r="F20">
-        <v>566</v>
+        <v>580</v>
       </c>
       <c r="G20">
         <v>527</v>
@@ -1314,14 +1195,8 @@
       <c r="J20">
         <v>0.90500000000000003</v>
       </c>
-      <c r="K20">
-        <v>0</v>
-      </c>
-      <c r="L20">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>25</v>
       </c>
@@ -1338,7 +1213,7 @@
         <v>2548</v>
       </c>
       <c r="F21">
-        <v>727</v>
+        <v>729</v>
       </c>
       <c r="G21">
         <v>563</v>
@@ -1352,14 +1227,8 @@
       <c r="J21">
         <v>0.878</v>
       </c>
-      <c r="K21">
-        <v>0</v>
-      </c>
-      <c r="L21">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>26</v>
       </c>
@@ -1376,7 +1245,7 @@
         <v>2505</v>
       </c>
       <c r="F22">
-        <v>802</v>
+        <v>808</v>
       </c>
       <c r="G22">
         <v>597</v>
@@ -1390,14 +1259,8 @@
       <c r="J22">
         <v>0.89300000000000002</v>
       </c>
-      <c r="K22">
-        <v>0</v>
-      </c>
-      <c r="L22">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>27</v>
       </c>
@@ -1428,19 +1291,13 @@
       <c r="J23">
         <v>0.89100000000000001</v>
       </c>
-      <c r="K23">
-        <v>0</v>
-      </c>
-      <c r="L23">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>28</v>
       </c>
       <c r="B24">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="C24">
         <v>40</v>
@@ -1452,7 +1309,7 @@
         <v>2522</v>
       </c>
       <c r="F24">
-        <v>558</v>
+        <v>562</v>
       </c>
       <c r="G24">
         <v>706</v>
@@ -1466,14 +1323,8 @@
       <c r="J24">
         <v>0.89700000000000002</v>
       </c>
-      <c r="K24">
-        <v>1</v>
-      </c>
-      <c r="L24">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>29</v>
       </c>
@@ -1490,7 +1341,7 @@
         <v>2257</v>
       </c>
       <c r="F25">
-        <v>617</v>
+        <v>627</v>
       </c>
       <c r="G25">
         <v>686</v>
@@ -1504,14 +1355,8 @@
       <c r="J25">
         <v>0.89500000000000002</v>
       </c>
-      <c r="K25">
-        <v>0</v>
-      </c>
-      <c r="L25">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>30</v>
       </c>
@@ -1528,7 +1373,7 @@
         <v>2045</v>
       </c>
       <c r="F26">
-        <v>741</v>
+        <v>745</v>
       </c>
       <c r="G26">
         <v>544</v>
@@ -1542,14 +1387,8 @@
       <c r="J26">
         <v>0.90200000000000002</v>
       </c>
-      <c r="K26">
-        <v>0</v>
-      </c>
-      <c r="L26">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>31</v>
       </c>
@@ -1566,7 +1405,7 @@
         <v>2238</v>
       </c>
       <c r="F27">
-        <v>540</v>
+        <v>542</v>
       </c>
       <c r="G27">
         <v>726</v>
@@ -1580,14 +1419,8 @@
       <c r="J27">
         <v>0.89500000000000002</v>
       </c>
-      <c r="K27">
-        <v>0</v>
-      </c>
-      <c r="L27">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>32</v>
       </c>
@@ -1618,14 +1451,8 @@
       <c r="J28">
         <v>0.90800000000000003</v>
       </c>
-      <c r="K28">
-        <v>0</v>
-      </c>
-      <c r="L28">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.3">
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>33</v>
       </c>
@@ -1656,14 +1483,8 @@
       <c r="J29">
         <v>0.9</v>
       </c>
-      <c r="K29">
-        <v>0</v>
-      </c>
-      <c r="L29">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.3">
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>34</v>
       </c>
@@ -1680,7 +1501,7 @@
         <v>2328</v>
       </c>
       <c r="F30">
-        <v>756</v>
+        <v>760</v>
       </c>
       <c r="G30">
         <v>499</v>
@@ -1694,14 +1515,8 @@
       <c r="J30">
         <v>0.91800000000000004</v>
       </c>
-      <c r="K30">
-        <v>0</v>
-      </c>
-      <c r="L30">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.3">
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>35</v>
       </c>
@@ -1732,14 +1547,8 @@
       <c r="J31">
         <v>0.89300000000000002</v>
       </c>
-      <c r="K31">
-        <v>0</v>
-      </c>
-      <c r="L31">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.3">
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>36</v>
       </c>
@@ -1769,12 +1578,6 @@
       </c>
       <c r="J32">
         <v>0.92700000000000005</v>
-      </c>
-      <c r="K32">
-        <v>0</v>
-      </c>
-      <c r="L32">
-        <v>0</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.3">

</xml_diff>